<commit_message>
Presentation added and changed rmd file
</commit_message>
<xml_diff>
--- a/Data/Fish_Production_UnitedStates.xlsx
+++ b/Data/Fish_Production_UnitedStates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4478aed3825114f0/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4478aed3825114f0/Desktop/Vallabh_Rutgers/Business Forecasting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{BCE77C56-5A31-404F-9694-1F1E268BB68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{653EC4DC-EA16-4219-8845-311684C9F64B}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{BCE77C56-5A31-404F-9694-1F1E268BB68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBCBEAC6-3363-457B-820E-E5C65F4B95B3}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="9456" yWindow="6876" windowWidth="12528" windowHeight="8964" xr2:uid="{51544C33-72AD-42C5-BEF3-41C087D19CEA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{51544C33-72AD-42C5-BEF3-41C087D19CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="6">
   <si>
     <t>Entity</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Year</t>
-  </si>
-  <si>
-    <t>Aquaculture production (metric tons)</t>
   </si>
   <si>
     <t>Capture fisheries production (metric tons)</t>
@@ -414,20 +411,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1FEEFD-094D-465C-8AD1-0B321A1DA2BF}">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,976 +436,802 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>1960</v>
       </c>
       <c r="D2">
-        <v>104421</v>
-      </c>
-      <c r="E2">
         <v>2714623</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>1961</v>
       </c>
       <c r="D3">
-        <v>102547</v>
-      </c>
-      <c r="E3">
         <v>2852004</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>1962</v>
       </c>
       <c r="D4">
-        <v>109961</v>
-      </c>
-      <c r="E4">
         <v>2897963</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>1963</v>
       </c>
       <c r="D5">
-        <v>122697</v>
-      </c>
-      <c r="E5">
         <v>2655052</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>1964</v>
       </c>
       <c r="D6">
-        <v>123884</v>
-      </c>
-      <c r="E6">
         <v>2519951</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>1965</v>
       </c>
       <c r="D7">
-        <v>132578</v>
-      </c>
-      <c r="E7">
         <v>2649980</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>1966</v>
       </c>
       <c r="D8">
-        <v>114236</v>
-      </c>
-      <c r="E8">
         <v>2442257</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>1967</v>
       </c>
       <c r="D9">
-        <v>127299</v>
-      </c>
-      <c r="E9">
         <v>2311726</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>1968</v>
       </c>
       <c r="D10">
-        <v>131115</v>
-      </c>
-      <c r="E10">
         <v>2410943</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>1969</v>
       </c>
       <c r="D11">
-        <v>116768</v>
-      </c>
-      <c r="E11">
         <v>2439130</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>1970</v>
       </c>
       <c r="D12">
-        <v>168681</v>
-      </c>
-      <c r="E12">
         <v>2794298</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <v>1971</v>
       </c>
       <c r="D13">
-        <v>165590</v>
-      </c>
-      <c r="E13">
         <v>2885230</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <v>1972</v>
       </c>
       <c r="D14">
-        <v>173630</v>
-      </c>
-      <c r="E14">
         <v>2772595</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>1973</v>
       </c>
       <c r="D15">
-        <v>170320</v>
-      </c>
-      <c r="E15">
         <v>2808362</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>1974</v>
       </c>
       <c r="D16">
-        <v>167039</v>
-      </c>
-      <c r="E16">
         <v>2885967</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>1975</v>
       </c>
       <c r="D17">
-        <v>218459</v>
-      </c>
-      <c r="E17">
         <v>2847282</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>1976</v>
       </c>
       <c r="D18">
-        <v>183907</v>
-      </c>
-      <c r="E18">
         <v>3088267</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <v>1977</v>
       </c>
       <c r="D19">
-        <v>174310</v>
-      </c>
-      <c r="E19">
         <v>3037617</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>1978</v>
       </c>
       <c r="D20">
-        <v>158795</v>
-      </c>
-      <c r="E20">
         <v>3477688</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21">
         <v>1979</v>
       </c>
       <c r="D21">
-        <v>138990</v>
-      </c>
-      <c r="E21">
         <v>3583385</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22">
         <v>1980</v>
       </c>
       <c r="D22">
-        <v>168365</v>
-      </c>
-      <c r="E22">
         <v>3703301</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23">
         <v>1981</v>
       </c>
       <c r="D23">
-        <v>230111</v>
-      </c>
-      <c r="E23">
         <v>3701137</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>1982</v>
       </c>
       <c r="D24">
-        <v>261725</v>
-      </c>
-      <c r="E24">
         <v>3952683</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25">
         <v>1983</v>
       </c>
       <c r="D25">
-        <v>268483</v>
-      </c>
-      <c r="E25">
         <v>4152983</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26">
         <v>1984</v>
       </c>
       <c r="D26">
-        <v>326453</v>
-      </c>
-      <c r="E26">
         <v>4721775</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27">
         <v>1985</v>
       </c>
       <c r="D27">
-        <v>323573</v>
-      </c>
-      <c r="E27">
         <v>4719868</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28">
         <v>1986</v>
       </c>
       <c r="D28">
-        <v>372191</v>
-      </c>
-      <c r="E28">
         <v>4880950</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29">
         <v>1987</v>
       </c>
       <c r="D29">
-        <v>383259</v>
-      </c>
-      <c r="E29">
         <v>5694242</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30">
         <v>1988</v>
       </c>
       <c r="D30">
-        <v>357657</v>
-      </c>
-      <c r="E30">
         <v>5670666</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <v>1989</v>
       </c>
       <c r="D31">
-        <v>369252</v>
-      </c>
-      <c r="E31">
         <v>5491353</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32">
         <v>1990</v>
       </c>
       <c r="D32">
-        <v>315727</v>
-      </c>
-      <c r="E32">
         <v>5620405</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33">
         <v>1991</v>
       </c>
       <c r="D33">
-        <v>363083</v>
-      </c>
-      <c r="E33">
         <v>5244569</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34">
         <v>1992</v>
       </c>
       <c r="D34">
-        <v>413844</v>
-      </c>
-      <c r="E34">
         <v>5274934</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35">
         <v>1993</v>
       </c>
       <c r="D35">
-        <v>416913</v>
-      </c>
-      <c r="E35">
         <v>5608158</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36">
         <v>1994</v>
       </c>
       <c r="D36">
-        <v>391412</v>
-      </c>
-      <c r="E36">
         <v>5652548</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C37">
         <v>1995</v>
       </c>
       <c r="D37">
-        <v>413454</v>
-      </c>
-      <c r="E37">
         <v>5299199</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38">
         <v>1996</v>
       </c>
       <c r="D38">
-        <v>393346</v>
-      </c>
-      <c r="E38">
         <v>5060701</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39">
         <v>1997</v>
       </c>
       <c r="D39">
-        <v>438356</v>
-      </c>
-      <c r="E39">
         <v>5054872</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40">
         <v>1998</v>
       </c>
       <c r="D40">
-        <v>445119</v>
-      </c>
-      <c r="E40">
         <v>4735868</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41">
         <v>1999</v>
       </c>
       <c r="D41">
-        <v>479212</v>
-      </c>
-      <c r="E41">
         <v>4831285</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>2000</v>
       </c>
       <c r="D42">
-        <v>456830</v>
-      </c>
-      <c r="E42">
         <v>4760000</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43">
         <v>2001</v>
       </c>
       <c r="D43">
-        <v>480362</v>
-      </c>
-      <c r="E43">
         <v>4981801</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C44">
         <v>2002</v>
       </c>
       <c r="D44">
-        <v>498899</v>
-      </c>
-      <c r="E44">
         <v>4984749</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45">
         <v>2003</v>
       </c>
       <c r="D45">
-        <v>545971</v>
-      </c>
-      <c r="E45">
         <v>4988681</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C46">
         <v>2004</v>
       </c>
       <c r="D46">
-        <v>607570</v>
-      </c>
-      <c r="E46">
         <v>4995418</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C47">
         <v>2005</v>
       </c>
       <c r="D47">
-        <v>513920</v>
-      </c>
-      <c r="E47">
         <v>4961267</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48">
         <v>2006</v>
       </c>
       <c r="D48">
-        <v>519967</v>
-      </c>
-      <c r="E48">
         <v>4858805</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C49">
         <v>2007</v>
       </c>
       <c r="D49">
-        <v>526045</v>
-      </c>
-      <c r="E49">
         <v>4770169</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C50">
         <v>2008</v>
       </c>
       <c r="D50">
-        <v>501326</v>
-      </c>
-      <c r="E50">
         <v>4360459</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C51">
         <v>2009</v>
       </c>
       <c r="D51">
-        <v>481224</v>
-      </c>
-      <c r="E51">
         <v>4233804</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C52">
         <v>2010</v>
       </c>
       <c r="D52">
-        <v>496699</v>
-      </c>
-      <c r="E52">
         <v>4396632</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C53">
         <v>2011</v>
       </c>
       <c r="D53">
-        <v>397292</v>
-      </c>
-      <c r="E53">
         <v>5123157</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C54">
         <v>2012</v>
       </c>
       <c r="D54">
-        <v>420386</v>
-      </c>
-      <c r="E54">
         <v>5100858</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C55">
         <v>2013</v>
       </c>
       <c r="D55">
-        <v>429011</v>
-      </c>
-      <c r="E55">
         <v>5153379</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C56">
         <v>2014</v>
       </c>
       <c r="D56">
-        <v>421189</v>
-      </c>
-      <c r="E56">
         <v>4984481</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C57">
         <v>2015</v>
       </c>
       <c r="D57">
-        <v>426002</v>
-      </c>
-      <c r="E57">
         <v>5045443</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C58">
         <v>2016</v>
       </c>
       <c r="D58">
-        <v>444369</v>
-      </c>
-      <c r="E58">
         <v>4931017</v>
       </c>
     </row>

</xml_diff>